<commit_message>
feat: license and readme updated
</commit_message>
<xml_diff>
--- a/example/sample.xlsx
+++ b/example/sample.xlsx
@@ -67,64 +67,64 @@
     <t>software</t>
   </si>
   <si>
-    <t>bandana</t>
-  </si>
-  <si>
-    <t>roshan</t>
-  </si>
-  <si>
-    <t>sanjay</t>
-  </si>
-  <si>
-    <t>rukesh</t>
-  </si>
-  <si>
-    <t>Aungush</t>
-  </si>
-  <si>
-    <t>nikesh</t>
-  </si>
-  <si>
-    <t>seena</t>
-  </si>
-  <si>
-    <t>santosh</t>
-  </si>
-  <si>
-    <t>pratik</t>
-  </si>
-  <si>
-    <t>jeena</t>
-  </si>
-  <si>
-    <t>rajani</t>
-  </si>
-  <si>
-    <t>haris</t>
-  </si>
-  <si>
-    <t>shreetika</t>
-  </si>
-  <si>
-    <t>prijal</t>
-  </si>
-  <si>
-    <t>samina</t>
-  </si>
-  <si>
-    <t>anish</t>
-  </si>
-  <si>
-    <t>rasil</t>
-  </si>
-  <si>
-    <t>amit</t>
-  </si>
-  <si>
-    <t>anjeela</t>
-  </si>
-  <si>
-    <t>sushmin</t>
+    <t>Kamran Bains</t>
+  </si>
+  <si>
+    <t>Chloe-Ann Vega</t>
+  </si>
+  <si>
+    <t>Amayah Barajas</t>
+  </si>
+  <si>
+    <t>Safa Blackburn</t>
+  </si>
+  <si>
+    <t>Kezia Gonzalez</t>
+  </si>
+  <si>
+    <t>Boyd Mcbride</t>
+  </si>
+  <si>
+    <t>Leela Romero</t>
+  </si>
+  <si>
+    <t>Mateusz Thornton</t>
+  </si>
+  <si>
+    <t>Amelie Bell</t>
+  </si>
+  <si>
+    <t>Jevon Myers</t>
+  </si>
+  <si>
+    <t>Riley-James Duran</t>
+  </si>
+  <si>
+    <t>Glen Churchill</t>
+  </si>
+  <si>
+    <t>Sachin Deacon</t>
+  </si>
+  <si>
+    <t>Rufus Redfern</t>
+  </si>
+  <si>
+    <t>Jonah Best</t>
+  </si>
+  <si>
+    <t>Zion Ingram</t>
+  </si>
+  <si>
+    <t>Matei Gibbs</t>
+  </si>
+  <si>
+    <t>Kaelan Mcdonnell</t>
+  </si>
+  <si>
+    <t>Spike Peel</t>
+  </si>
+  <si>
+    <t>Zakariyah Gray</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
fix: fix issue of empty sheet data and missing non optional sheet data
</commit_message>
<xml_diff>
--- a/example/sample.xlsx
+++ b/example/sample.xlsx
@@ -5,6 +5,7 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="First sheet" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="second sheet" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -698,4 +699,14 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>